<commit_message>
msz - and even more demo app work - new radiobutton control
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED86519F-7B2C-4802-9C2A-B78AEEAC3005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4D5B82-9E02-4BE3-A489-DBA51735EA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1188" yWindow="2940" windowWidth="35280" windowHeight="13512" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="35280" windowHeight="13512" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Action</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>&lt;NOTSELECTED&gt;</t>
+  </si>
+  <si>
+    <t>102_VehicleInsuranceAutomobile_001_SmokeTest_FillPageInsurantData</t>
+  </si>
+  <si>
+    <t>Goto insurant page</t>
+  </si>
+  <si>
+    <t>&lt;SELECT&gt;</t>
+  </si>
+  <si>
+    <t>Button Next from Page VehicleData</t>
+  </si>
+  <si>
+    <t>Button Next</t>
   </si>
 </sst>
 </file>
@@ -183,14 +198,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>144781</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>212057</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>121921</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>83821</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -213,7 +228,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3474721"/>
+          <a:off x="0" y="1973581"/>
           <a:ext cx="8594057" cy="5059680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -523,18 +538,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="60" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.88671875" customWidth="1"/>
+    <col min="3" max="4" width="50" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.77734375" customWidth="1"/>
     <col min="6" max="6" width="32.44140625" customWidth="1"/>
     <col min="7" max="7" width="20.5546875" customWidth="1"/>
@@ -636,15 +650,57 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
msz - first smoke test is running
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4D5B82-9E02-4BE3-A489-DBA51735EA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242BF836-D7F5-46BA-93E0-82CE411FEF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="35280" windowHeight="13512" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="1320" yWindow="756" windowWidth="35280" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>Action</t>
   </si>
@@ -115,6 +115,33 @@
   </si>
   <si>
     <t>Button Next</t>
+  </si>
+  <si>
+    <t>102_VehicleInsuranceAutomobile_001_SmokeTest_FillPageProductData</t>
+  </si>
+  <si>
+    <t>Choose Silver</t>
+  </si>
+  <si>
+    <t>Choose Gold</t>
+  </si>
+  <si>
+    <t>Choose Platinum</t>
+  </si>
+  <si>
+    <t>Choose Ultimate</t>
+  </si>
+  <si>
+    <t>Goto product page</t>
+  </si>
+  <si>
+    <t>102_VehicleInsuranceAutomobile_001_SmokeTest_FillPageSendQuote</t>
+  </si>
+  <si>
+    <t>Send Quote - Button Main Page</t>
+  </si>
+  <si>
+    <t>Button Main Page</t>
   </si>
 </sst>
 </file>
@@ -198,14 +225,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>144781</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>99061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>212057</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>83821</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -228,7 +255,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1973581"/>
+          <a:off x="0" y="3025141"/>
           <a:ext cx="8594057" cy="5059680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -538,20 +565,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="60" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="4" width="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+    <col min="3" max="5" width="50" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.44140625" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" customWidth="1"/>
+    <col min="7" max="7" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -664,26 +690,23 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>4</v>
+      <c r="E6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="H7" t="s">
@@ -692,15 +715,127 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
         <v>29</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
msz - mandatory fields checks part 1
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AE66A4-1DC4-4C12-882C-DE494524E095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7377B3A-35CB-42F0-BF05-A26E71F28FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9972" yWindow="1968" windowWidth="29856" windowHeight="12480" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="37836" windowHeight="14088" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
   <si>
     <t>Action</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>old_102_VehicleInsuranceAutomobile_001_SmokeTest_FillPageSendQuote</t>
+  </si>
+  <si>
+    <t>Vehicle Page check for open mandatory fields</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_002_VehicleData_001_MandatoryFields_FillMake</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_002_VehicleData_001_MandatoryFields_CheckFilledMake</t>
   </si>
 </sst>
 </file>
@@ -244,14 +253,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>83821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>212057</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2848577</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>22861</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -274,7 +283,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3025141"/>
+          <a:off x="0" y="4290061"/>
           <a:ext cx="8594057" cy="5059680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -584,17 +593,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="5" width="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="50" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.44140625" customWidth="1"/>
     <col min="7" max="7" width="50" bestFit="1" customWidth="1"/>
   </cols>
@@ -858,6 +868,48 @@
         <v>4</v>
       </c>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
msz - mandatory field checks part 3 incl. groupbox
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7377B3A-35CB-42F0-BF05-A26E71F28FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C55364-1179-4478-9112-5A9C99043A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="37836" windowHeight="14088" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="5340" yWindow="984" windowWidth="32112" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="50">
   <si>
     <t>Action</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>102_AutomobileInsurance_002_VehicleData_001_MandatoryFields_CheckFilledMake</t>
+  </si>
+  <si>
+    <t>//*[@id="enterinsurantdata"]</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_003_InsurantData_001_MandatoryFields_FillFirstName</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_003_InsurantData_001_MandatoryFields_CheckFilledFirstName</t>
+  </si>
+  <si>
+    <t>Insurant Page check for open mandatory fields</t>
   </si>
 </sst>
 </file>
@@ -253,13 +265,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>83821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2848577</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:colOff>2437097</xdr:colOff>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>22861</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -593,18 +605,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.5546875" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
     <col min="3" max="3" width="71.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.44140625" customWidth="1"/>
     <col min="7" max="7" width="50" bestFit="1" customWidth="1"/>
   </cols>
@@ -620,7 +633,7 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>19</v>
@@ -643,7 +656,9 @@
         <v>7</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -907,6 +922,48 @@
         <v>45</v>
       </c>
       <c r="H19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
msz - field hint and error checks part 1
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C55364-1179-4478-9112-5A9C99043A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C6F59B-4098-491B-9D04-6CFD36A5C89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="984" windowWidth="32112" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="456" yWindow="1344" windowWidth="37164" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
   <si>
     <t>Action</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Insurant Page check for open mandatory fields</t>
+  </si>
+  <si>
+    <t>Vehicle Page check for hints regarding mandatory fields</t>
   </si>
 </sst>
 </file>
@@ -605,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,6 +970,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
msz - field hint and error checks part 2
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C6F59B-4098-491B-9D04-6CFD36A5C89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2AB7A2-873D-4132-8C7A-41B74D32F4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="456" yWindow="1344" windowWidth="37164" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="456" yWindow="960" windowWidth="37164" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
   <si>
     <t>Action</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>Vehicle Page check for hints regarding mandatory fields</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_002_VehicleData_002_EnterNumericValuesBelowRange</t>
+  </si>
+  <si>
+    <t>Vehicle Page check error hint list value ranges</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_002_VehicleData_002_EnterNumericValuesAboveRange</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_002_VehicleData_002_ManufacturingDateInTheFuture</t>
+  </si>
+  <si>
+    <t>Vehicle Page check error hint manufacturing date in the future</t>
   </si>
 </sst>
 </file>
@@ -268,14 +283,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>83821</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>60961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2437097</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>22861</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -298,7 +313,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="4290061"/>
+          <a:off x="0" y="5364481"/>
           <a:ext cx="8594057" cy="5059680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -608,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,6 +999,76 @@
         <v>4</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
msz - field hint and error checks part 3 + listener experiments
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2AB7A2-873D-4132-8C7A-41B74D32F4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E1A8A2-AAE9-49F4-9DAB-A81B63BDB8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="456" yWindow="960" windowWidth="37164" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="1632" yWindow="624" windowWidth="37164" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="61">
   <si>
     <t>Action</t>
   </si>
@@ -193,6 +193,21 @@
   </si>
   <si>
     <t>Vehicle Page check error hint manufacturing date in the future</t>
+  </si>
+  <si>
+    <t>Insurant Page check for hints regarding mandatory fields</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_003_InsurantData_002_EnterValuesInWrongFormat</t>
+  </si>
+  <si>
+    <t>Insurant Page check error hint formatting</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_003_InsurantData_002_EnterValuesInWrongFormat Part 2</t>
+  </si>
+  <si>
+    <t>Insurant Page check error hint formatting Part 2</t>
   </si>
 </sst>
 </file>
@@ -283,14 +298,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>60961</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>99061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2437097</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -313,7 +328,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="5364481"/>
+          <a:off x="0" y="6316981"/>
           <a:ext cx="8594057" cy="5059680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -623,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -945,13 +960,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="D20" t="s">
-        <v>49</v>
+      <c r="C20" t="s">
+        <v>50</v>
       </c>
       <c r="H20" t="s">
         <v>4</v>
@@ -959,13 +974,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>47</v>
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
       </c>
       <c r="H21" t="s">
         <v>4</v>
@@ -973,13 +988,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>48</v>
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
       </c>
       <c r="H22" t="s">
         <v>4</v>
@@ -987,13 +1002,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H23" t="s">
         <v>4</v>
@@ -1001,13 +1016,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H24" t="s">
         <v>4</v>
@@ -1015,13 +1030,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H25" t="s">
         <v>4</v>
@@ -1029,13 +1044,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>53</v>
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
       </c>
       <c r="H26" t="s">
         <v>4</v>
@@ -1043,13 +1058,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
-      <c r="C27" t="s">
-        <v>54</v>
+      <c r="D27" t="s">
+        <v>47</v>
       </c>
       <c r="H27" t="s">
         <v>4</v>
@@ -1057,15 +1072,85 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
-      <c r="C28" t="s">
-        <v>55</v>
+      <c r="D28" t="s">
+        <v>48</v>
       </c>
       <c r="H28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>56</v>
+      </c>
+      <c r="H29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H33" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
msz - field hint and error checks part 4 + dialog resolve
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E1A8A2-AAE9-49F4-9DAB-A81B63BDB8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBD5E6E-CE83-4D18-B469-3C15C5EFAE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1632" yWindow="624" windowWidth="37164" windowHeight="15720" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="1632" yWindow="156" windowWidth="39024" windowHeight="14352" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="62">
   <si>
     <t>Action</t>
   </si>
@@ -165,9 +165,6 @@
     <t>102_AutomobileInsurance_002_VehicleData_001_MandatoryFields_CheckFilledMake</t>
   </si>
   <si>
-    <t>//*[@id="enterinsurantdata"]</t>
-  </si>
-  <si>
     <t>102_AutomobileInsurance_003_InsurantData_001_MandatoryFields_FillFirstName</t>
   </si>
   <si>
@@ -208,6 +205,12 @@
   </si>
   <si>
     <t>Insurant Page check error hint formatting Part 2</t>
+  </si>
+  <si>
+    <t>Product Page check for open mandatory fields</t>
+  </si>
+  <si>
+    <t>Product Page check for filled mandatory fields</t>
   </si>
 </sst>
 </file>
@@ -298,14 +301,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>137161</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2437097</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -328,7 +331,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="6316981"/>
+          <a:off x="0" y="6720841"/>
           <a:ext cx="8594057" cy="5059680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -638,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,8 +668,8 @@
       <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
-        <v>46</v>
+      <c r="D1" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>19</v>
@@ -960,13 +963,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" t="s">
         <v>4</v>
@@ -974,13 +977,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H21" t="s">
         <v>4</v>
@@ -988,13 +991,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" t="s">
         <v>4</v>
@@ -1002,13 +1005,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23" t="s">
         <v>4</v>
@@ -1016,13 +1019,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H24" t="s">
         <v>4</v>
@@ -1030,13 +1033,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H25" t="s">
         <v>4</v>
@@ -1044,13 +1047,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H26" t="s">
         <v>4</v>
@@ -1058,13 +1061,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H27" t="s">
         <v>4</v>
@@ -1072,13 +1075,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H28" t="s">
         <v>4</v>
@@ -1086,13 +1089,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H29" t="s">
         <v>4</v>
@@ -1100,13 +1103,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H30" t="s">
         <v>4</v>
@@ -1114,13 +1117,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H31" t="s">
         <v>4</v>
@@ -1128,13 +1131,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H32" t="s">
         <v>4</v>
@@ -1142,15 +1145,43 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>59</v>
+      </c>
+      <c r="H33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>60</v>
       </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
         <v>60</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
msz - bugfixes (web seems stable, still some flakiness in mobile tests)
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBD5E6E-CE83-4D18-B469-3C15C5EFAE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14B316F-6D8D-4B3A-8A1A-E649DEA3791F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1632" yWindow="156" windowWidth="39024" windowHeight="14352" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="2172" yWindow="888" windowWidth="34512" windowHeight="14352" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="63">
   <si>
     <t>Action</t>
   </si>
@@ -78,21 +78,9 @@
     <t>102_VehicleInsuranceAutomobile_001_SmokeTest_FillPage</t>
   </si>
   <si>
-    <t>//*[@id="insurance-form"]/div/section[1]</t>
-  </si>
-  <si>
     <t>//*[@id="insurance-form"]/div/section[2]</t>
   </si>
   <si>
-    <t>//*[@id="insurance-form"]/div/section[3]</t>
-  </si>
-  <si>
-    <t>//*[@id="insurance-form"]/div/section[4]</t>
-  </si>
-  <si>
-    <t>//*[@id="insurance-form"]/div/section[5]</t>
-  </si>
-  <si>
     <t>&lt;SELECTED&gt;</t>
   </si>
   <si>
@@ -211,6 +199,21 @@
   </si>
   <si>
     <t>Product Page check for filled mandatory fields</t>
+  </si>
+  <si>
+    <t>//*[@id='insurance-form']/div/section[1]</t>
+  </si>
+  <si>
+    <t>//*[@id='insurance-form']/div/section[2]</t>
+  </si>
+  <si>
+    <t>//*[@id='insurance-form']/div/section[3]</t>
+  </si>
+  <si>
+    <t>//*[@id='insurance-form']/div/section[4]</t>
+  </si>
+  <si>
+    <t>//*[@id='insurance-form']/div/section[5]</t>
   </si>
 </sst>
 </file>
@@ -272,12 +275,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -643,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,19 +670,19 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -693,7 +697,7 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -736,19 +740,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -756,13 +760,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
@@ -770,18 +774,18 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -795,7 +799,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -809,7 +813,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -823,7 +827,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -837,13 +841,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H11" t="s">
         <v>4</v>
@@ -851,13 +855,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H12" t="s">
         <v>4</v>
@@ -865,13 +869,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H13" t="s">
         <v>4</v>
@@ -879,13 +883,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H14" t="s">
         <v>4</v>
@@ -893,13 +897,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H15" t="s">
         <v>4</v>
@@ -907,13 +911,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
@@ -921,13 +925,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H17" t="s">
         <v>4</v>
@@ -935,13 +939,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H18" t="s">
         <v>4</v>
@@ -949,13 +953,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H19" t="s">
         <v>4</v>
@@ -963,13 +967,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H20" t="s">
         <v>4</v>
@@ -977,13 +981,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H21" t="s">
         <v>4</v>
@@ -991,13 +995,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H22" t="s">
         <v>4</v>
@@ -1005,13 +1009,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H23" t="s">
         <v>4</v>
@@ -1019,13 +1023,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H24" t="s">
         <v>4</v>
@@ -1033,13 +1037,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H25" t="s">
         <v>4</v>
@@ -1047,13 +1051,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H26" t="s">
         <v>4</v>
@@ -1061,13 +1065,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H27" t="s">
         <v>4</v>
@@ -1075,13 +1079,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H28" t="s">
         <v>4</v>
@@ -1089,13 +1093,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H29" t="s">
         <v>4</v>
@@ -1103,13 +1107,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H30" t="s">
         <v>4</v>
@@ -1117,13 +1121,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H31" t="s">
         <v>4</v>
@@ -1131,13 +1135,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H32" t="s">
         <v>4</v>
@@ -1145,13 +1149,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H33" t="s">
         <v>4</v>
@@ -1159,13 +1163,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H34" t="s">
         <v>4</v>
@@ -1173,13 +1177,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H35" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
msz - table part 1
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14B316F-6D8D-4B3A-8A1A-E649DEA3791F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770CFA79-B9E0-41A6-81DE-FDA1C08A4CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2172" yWindow="888" windowWidth="34512" windowHeight="14352" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="2520" yWindow="1236" windowWidth="34512" windowHeight="14352" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="70">
   <si>
     <t>Action</t>
   </si>
@@ -214,6 +214,27 @@
   </si>
   <si>
     <t>//*[@id='insurance-form']/div/section[5]</t>
+  </si>
+  <si>
+    <t>Product Page check for hints regarding mandatory fields</t>
+  </si>
+  <si>
+    <t>Product Page check for hint date with invalid format</t>
+  </si>
+  <si>
+    <t>Product Page check for hint date with invalid value in past</t>
+  </si>
+  <si>
+    <t>Product Page enter date with invalid format</t>
+  </si>
+  <si>
+    <t>Product Page enter date with invalid value in past</t>
+  </si>
+  <si>
+    <t>Price option page check for open mandatory field</t>
+  </si>
+  <si>
+    <t>Price option page check for filled mandatory field</t>
   </si>
 </sst>
 </file>
@@ -275,13 +296,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -305,14 +325,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>137161</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>160021</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2437097</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>99061</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -335,7 +355,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="6720841"/>
+          <a:off x="0" y="8023861"/>
           <a:ext cx="8594057" cy="5059680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -645,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,7 +678,7 @@
     <col min="3" max="3" width="71.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -672,7 +692,7 @@
       <c r="C1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" t="s">
         <v>59</v>
       </c>
       <c r="E1" t="s">
@@ -1186,6 +1206,104 @@
         <v>57</v>
       </c>
       <c r="H35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>65</v>
+      </c>
+      <c r="H40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" t="s">
+        <v>68</v>
+      </c>
+      <c r="H41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
msz - video 5 including today keyword
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770CFA79-B9E0-41A6-81DE-FDA1C08A4CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ECF022-97FF-4FDB-AAA4-B527093798BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="1236" windowWidth="34512" windowHeight="14352" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="2688" yWindow="1692" windowWidth="31740" windowHeight="14352" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="71">
   <si>
     <t>Action</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Price option page check for filled mandatory field</t>
+  </si>
+  <si>
+    <t>Price Option Page check for hints regarding mandatory fields</t>
   </si>
 </sst>
 </file>
@@ -665,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,7 +681,7 @@
     <col min="3" max="3" width="71.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1307,6 +1310,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>70</v>
+      </c>
+      <c r="H43" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
msz - more testcases including control changes + new infrastructure dir
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgAutomobileInsurance.xlsx
+++ b/Data/Dialogs/dlgAutomobileInsurance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ECF022-97FF-4FDB-AAA4-B527093798BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3503D2B4-7D35-4F05-AC49-D3214C3D0046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="1692" windowWidth="31740" windowHeight="14352" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="3720" yWindow="780" windowWidth="36948" windowHeight="15672" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="77">
   <si>
     <t>Action</t>
   </si>
@@ -238,6 +238,24 @@
   </si>
   <si>
     <t>Price Option Page check for hints regarding mandatory fields</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_006_SendQuote_002_EnterValuesInWrongFormat</t>
+  </si>
+  <si>
+    <t>102_AutomobileInsurance_006_SendQuote_002_EnterValuesInWrongFormat Part 2</t>
+  </si>
+  <si>
+    <t>Send Quote Page check error hint formatting Part 2</t>
+  </si>
+  <si>
+    <t>Send Quote Page check error hint formatting</t>
+  </si>
+  <si>
+    <t>Send Quote page check for open mandatory field</t>
+  </si>
+  <si>
+    <t>Send Quote Page check for hints regarding mandatory fields</t>
   </si>
 </sst>
 </file>
@@ -328,14 +346,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>160021</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2437097</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>160021</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -358,7 +376,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="8023861"/>
+          <a:off x="0" y="9364981"/>
           <a:ext cx="8594057" cy="5059680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -668,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1324,6 +1342,90 @@
         <v>4</v>
       </c>
     </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>75</v>
+      </c>
+      <c r="H44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>76</v>
+      </c>
+      <c r="H45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H49" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>